<commit_message>
Initial Commit Changing Column Names
</commit_message>
<xml_diff>
--- a/1150.xlsx
+++ b/1150.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sachithk\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yasirup\PycharmProjects\dfn_guys_backend\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20496" windowHeight="7752"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -29,30 +29,18 @@
     <t>Time</t>
   </si>
   <si>
-    <t xml:space="preserve"> Open</t>
-  </si>
-  <si>
     <t xml:space="preserve"> High</t>
   </si>
   <si>
     <t xml:space="preserve"> Low</t>
   </si>
   <si>
-    <t xml:space="preserve"> Close</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Volume</t>
   </si>
   <si>
     <t xml:space="preserve"> Turnover</t>
   </si>
   <si>
-    <t xml:space="preserve"> Chg.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> % Chg.</t>
-  </si>
-  <si>
     <t xml:space="preserve"> 31/12/2019 </t>
   </si>
   <si>
@@ -801,6 +789,18 @@
   </si>
   <si>
     <t xml:space="preserve"> 01/01/2019 </t>
+  </si>
+  <si>
+    <t>PctChg</t>
+  </si>
+  <si>
+    <t>Chg</t>
+  </si>
+  <si>
+    <t>Close</t>
+  </si>
+  <si>
+    <t>Open</t>
   </si>
 </sst>
 </file>
@@ -1121,47 +1121,47 @@
   <dimension ref="A1:I251"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD251"/>
+      <selection activeCell="O15" sqref="O15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="23" customWidth="1"/>
     <col min="7" max="7" width="26" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>258</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
+        <v>257</v>
+      </c>
+      <c r="F1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
+        <v>256</v>
+      </c>
+      <c r="I1" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
         <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>9</v>
       </c>
       <c r="B2">
         <v>24.879999160000001</v>
@@ -1188,9 +1188,9 @@
         <v>1.89</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B3">
         <v>25.350000380000001</v>
@@ -1217,9 +1217,9 @@
         <v>-2.0499999999999998</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B4">
         <v>25.700000760000002</v>
@@ -1246,9 +1246,9 @@
         <v>-1.17</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B5">
         <v>25.799999239999998</v>
@@ -1275,9 +1275,9 @@
         <v>-0.39</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B6">
         <v>25.799999239999998</v>
@@ -1304,9 +1304,9 @@
         <v>-0.19</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B7">
         <v>25.899999619999999</v>
@@ -1333,9 +1333,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B8">
         <v>25.799999239999998</v>
@@ -1362,9 +1362,9 @@
         <v>0.19</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B9">
         <v>25.899999619999999</v>
@@ -1391,9 +1391,9 @@
         <v>-0.57999999999999996</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B10">
         <v>26.100000380000001</v>
@@ -1420,9 +1420,9 @@
         <v>-0.56999999999999995</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B11">
         <v>25.899999619999999</v>
@@ -1449,9 +1449,9 @@
         <v>0.38</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B12">
         <v>26.049999239999998</v>
@@ -1478,9 +1478,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B13">
         <v>25.799999239999998</v>
@@ -1507,9 +1507,9 @@
         <v>1.56</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B14">
         <v>25.049999239999998</v>
@@ -1536,9 +1536,9 @@
         <v>6.49</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B15">
         <v>24.36000061</v>
@@ -1565,9 +1565,9 @@
         <v>-1.31</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B16">
         <v>24</v>
@@ -1594,9 +1594,9 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B17">
         <v>24.059999470000001</v>
@@ -1623,9 +1623,9 @@
         <v>-0.66</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B18">
         <v>24.100000380000001</v>
@@ -1652,9 +1652,9 @@
         <v>0.67</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B19">
         <v>23.079999919999999</v>
@@ -1681,9 +1681,9 @@
         <v>3.99</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B20">
         <v>23</v>
@@ -1710,9 +1710,9 @@
         <v>0.17</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B21">
         <v>23.100000380000001</v>
@@ -1739,9 +1739,9 @@
         <v>-0.26</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B22">
         <v>22.879999160000001</v>
@@ -1768,9 +1768,9 @@
         <v>0.87</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B23">
         <v>22.979999540000001</v>
@@ -1797,9 +1797,9 @@
         <v>-0.35</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B24">
         <v>22.86000061</v>
@@ -1826,9 +1826,9 @@
         <v>0.79</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B25">
         <v>22.600000380000001</v>
@@ -1855,9 +1855,9 @@
         <v>0.97</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B26">
         <v>22.81999969</v>
@@ -1884,9 +1884,9 @@
         <v>-1.57</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B27">
         <v>22.86000061</v>
@@ -1913,9 +1913,9 @@
         <v>0.26</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B28">
         <v>22.760000229999999</v>
@@ -1942,9 +1942,9 @@
         <v>0.35</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B29">
         <v>23</v>
@@ -1971,9 +1971,9 @@
         <v>-0.87</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="B30">
         <v>22.879999160000001</v>
@@ -2000,9 +2000,9 @@
         <v>0.44</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="B31">
         <v>22.879999160000001</v>
@@ -2029,9 +2029,9 @@
         <v>0.17</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B32">
         <v>22.659999849999998</v>
@@ -2058,9 +2058,9 @@
         <v>1.1499999999999999</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B33">
         <v>22.299999239999998</v>
@@ -2087,9 +2087,9 @@
         <v>1.53</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="B34">
         <v>22.059999470000001</v>
@@ -2116,9 +2116,9 @@
         <v>0.91</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="B35">
         <v>22.059999470000001</v>
@@ -2145,9 +2145,9 @@
         <v>-0.36</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="B36">
         <v>22</v>
@@ -2174,9 +2174,9 @@
         <v>0.64</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B37">
         <v>21.86000061</v>
@@ -2203,9 +2203,9 @@
         <v>0.64</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B38">
         <v>21.799999239999998</v>
@@ -2232,9 +2232,9 @@
         <v>0.64</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B39">
         <v>21.200000760000002</v>
@@ -2261,9 +2261,9 @@
         <v>2.94</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B40">
         <v>20.86000061</v>
@@ -2290,9 +2290,9 @@
         <v>0.96</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B41">
         <v>21.200000760000002</v>
@@ -2319,9 +2319,9 @@
         <v>-1.23</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B42">
         <v>21.13999939</v>
@@ -2348,9 +2348,9 @@
         <v>0.28000000000000003</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B43">
         <v>20.899999619999999</v>
@@ -2377,9 +2377,9 @@
         <v>1.25</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="B44">
         <v>20.700000760000002</v>
@@ -2406,9 +2406,9 @@
         <v>-0.56999999999999995</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B45">
         <v>21.13999939</v>
@@ -2435,9 +2435,9 @@
         <v>-0.85</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="B46">
         <v>20.63999939</v>
@@ -2464,9 +2464,9 @@
         <v>2.2200000000000002</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B47">
         <v>21.020000459999999</v>
@@ -2493,9 +2493,9 @@
         <v>-1.99</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="B48">
         <v>21.459999079999999</v>
@@ -2522,9 +2522,9 @@
         <v>-1.95</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B49">
         <v>21.68000031</v>
@@ -2551,9 +2551,9 @@
         <v>-0.83</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B50">
         <v>21.799999239999998</v>
@@ -2580,9 +2580,9 @@
         <v>-0.37</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B51">
         <v>21.520000459999999</v>
@@ -2609,9 +2609,9 @@
         <v>1.3</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B52">
         <v>20.840000150000002</v>
@@ -2638,9 +2638,9 @@
         <v>4.88</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B53">
         <v>20.799999239999998</v>
@@ -2667,9 +2667,9 @@
         <v>-1.06</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="B54">
         <v>20.5</v>
@@ -2696,9 +2696,9 @@
         <v>3.39</v>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B55">
         <v>20.100000380000001</v>
@@ -2725,9 +2725,9 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="B56">
         <v>19.700000760000002</v>
@@ -2754,9 +2754,9 @@
         <v>1.52</v>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B57">
         <v>20.040000920000001</v>
@@ -2783,9 +2783,9 @@
         <v>-1.5</v>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B58">
         <v>20.340000150000002</v>
@@ -2812,9 +2812,9 @@
         <v>-0.99</v>
       </c>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="B59">
         <v>20.479999540000001</v>
@@ -2841,9 +2841,9 @@
         <v>-1.27</v>
       </c>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B60">
         <v>20.600000380000001</v>
@@ -2870,9 +2870,9 @@
         <v>-0.78</v>
       </c>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="B61">
         <v>21.260000229999999</v>
@@ -2899,9 +2899,9 @@
         <v>-3.01</v>
       </c>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="B62">
         <v>21.5</v>
@@ -2928,9 +2928,9 @@
         <v>-1.1200000000000001</v>
       </c>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="B63">
         <v>21.81999969</v>
@@ -2957,9 +2957,9 @@
         <v>-1.47</v>
       </c>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="B64">
         <v>22.020000459999999</v>
@@ -2986,9 +2986,9 @@
         <v>-0.09</v>
       </c>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B65">
         <v>21.899999619999999</v>
@@ -3015,9 +3015,9 @@
         <v>-0.73</v>
       </c>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="B66">
         <v>22.200000760000002</v>
@@ -3044,9 +3044,9 @@
         <v>-1.08</v>
       </c>
     </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B67">
         <v>22.600000380000001</v>
@@ -3073,9 +3073,9 @@
         <v>-1.07</v>
       </c>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="B68">
         <v>22.36000061</v>
@@ -3102,9 +3102,9 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="B69">
         <v>22.079999919999999</v>
@@ -3131,9 +3131,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B70">
         <v>22.020000459999999</v>
@@ -3160,9 +3160,9 @@
         <v>0.18</v>
       </c>
     </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B71">
         <v>22.200000760000002</v>
@@ -3189,9 +3189,9 @@
         <v>-0.72</v>
       </c>
     </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="B72">
         <v>21.920000080000001</v>
@@ -3218,9 +3218,9 @@
         <v>1.28</v>
       </c>
     </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="B73">
         <v>21.879999160000001</v>
@@ -3247,9 +3247,9 @@
         <v>0.09</v>
       </c>
     </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="B74">
         <v>21.420000080000001</v>
@@ -3276,9 +3276,9 @@
         <v>1.96</v>
       </c>
     </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="B75">
         <v>21.799999239999998</v>
@@ -3305,9 +3305,9 @@
         <v>-0.92</v>
       </c>
     </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="B76">
         <v>21.600000380000001</v>
@@ -3334,9 +3334,9 @@
         <v>0.28000000000000003</v>
       </c>
     </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="B77">
         <v>21.440000529999999</v>
@@ -3363,9 +3363,9 @@
         <v>0.93</v>
       </c>
     </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="B78">
         <v>20.899999619999999</v>
@@ -3392,9 +3392,9 @@
         <v>0.28000000000000003</v>
       </c>
     </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="B79">
         <v>21.18000031</v>
@@ -3421,9 +3421,9 @@
         <v>0.56999999999999995</v>
       </c>
     </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="B80">
         <v>21.780000690000001</v>
@@ -3450,9 +3450,9 @@
         <v>-2.57</v>
       </c>
     </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="B81">
         <v>22.079999919999999</v>
@@ -3479,9 +3479,9 @@
         <v>-1.36</v>
       </c>
     </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="B82">
         <v>22.100000380000001</v>
@@ -3508,9 +3508,9 @@
         <v>-0.18</v>
       </c>
     </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="B83">
         <v>22.120000839999999</v>
@@ -3537,9 +3537,9 @@
         <v>0.27</v>
       </c>
     </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="B84">
         <v>22.219999309999999</v>
@@ -3566,9 +3566,9 @@
         <v>-0.45</v>
       </c>
     </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="B85">
         <v>21.940000529999999</v>
@@ -3595,9 +3595,9 @@
         <v>1.19</v>
       </c>
     </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="B86">
         <v>22.059999470000001</v>
@@ -3624,9 +3624,9 @@
         <v>-0.82</v>
       </c>
     </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="B87">
         <v>21.81999969</v>
@@ -3653,9 +3653,9 @@
         <v>1.28</v>
       </c>
     </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="B88">
         <v>22</v>
@@ -3682,9 +3682,9 @@
         <v>-0.91</v>
       </c>
     </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="B89">
         <v>22.31999969</v>
@@ -3711,9 +3711,9 @@
         <v>-1.43</v>
       </c>
     </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="B90">
         <v>22.5</v>
@@ -3740,9 +3740,9 @@
         <v>-1.59</v>
       </c>
     </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="B91">
         <v>23.219999309999999</v>
@@ -3769,9 +3769,9 @@
         <v>-1.48</v>
       </c>
     </row>
-    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="B92">
         <v>22.840000150000002</v>
@@ -3798,9 +3798,9 @@
         <v>0.88</v>
       </c>
     </row>
-    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="B93">
         <v>23.600000380000001</v>
@@ -3827,9 +3827,9 @@
         <v>-4.04</v>
       </c>
     </row>
-    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="B94">
         <v>23.920000080000001</v>
@@ -3856,9 +3856,9 @@
         <v>-0.67</v>
       </c>
     </row>
-    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="B95">
         <v>24.100000380000001</v>
@@ -3885,9 +3885,9 @@
         <v>-0.57999999999999996</v>
       </c>
     </row>
-    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="B96">
         <v>24.219999309999999</v>
@@ -3914,9 +3914,9 @@
         <v>-0.5</v>
       </c>
     </row>
-    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="B97">
         <v>24.100000380000001</v>
@@ -3943,9 +3943,9 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="B98">
         <v>24.13999939</v>
@@ -3972,9 +3972,9 @@
         <v>-1.1499999999999999</v>
       </c>
     </row>
-    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="B99">
         <v>24.36000061</v>
@@ -4001,9 +4001,9 @@
         <v>-0.65</v>
       </c>
     </row>
-    <row r="100" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="B100">
         <v>24.399999619999999</v>
@@ -4030,9 +4030,9 @@
         <v>0.49</v>
       </c>
     </row>
-    <row r="101" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="B101">
         <v>24.159999849999998</v>
@@ -4059,9 +4059,9 @@
         <v>0.08</v>
       </c>
     </row>
-    <row r="102" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="B102">
         <v>24.879999160000001</v>
@@ -4088,9 +4088,9 @@
         <v>-2.25</v>
       </c>
     </row>
-    <row r="103" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="B103">
         <v>24.600000380000001</v>
@@ -4117,9 +4117,9 @@
         <v>0.32</v>
       </c>
     </row>
-    <row r="104" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="B104">
         <v>24.879999160000001</v>
@@ -4146,9 +4146,9 @@
         <v>-1.39</v>
       </c>
     </row>
-    <row r="105" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="B105">
         <v>24.879999160000001</v>
@@ -4175,9 +4175,9 @@
         <v>1.25</v>
       </c>
     </row>
-    <row r="106" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="B106">
         <v>25</v>
@@ -4204,9 +4204,9 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="107" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="B107">
         <v>25.549999239999998</v>
@@ -4233,9 +4233,9 @@
         <v>-3.74</v>
       </c>
     </row>
-    <row r="108" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="B108">
         <v>25.450000760000002</v>
@@ -4262,9 +4262,9 @@
         <v>0.78</v>
       </c>
     </row>
-    <row r="109" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="B109">
         <v>25.350000380000001</v>
@@ -4291,9 +4291,9 @@
         <v>0.79</v>
       </c>
     </row>
-    <row r="110" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="B110">
         <v>25.299999239999998</v>
@@ -4320,9 +4320,9 @@
         <v>-0.2</v>
       </c>
     </row>
-    <row r="111" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="B111">
         <v>25.700000760000002</v>
@@ -4349,9 +4349,9 @@
         <v>-1.74</v>
       </c>
     </row>
-    <row r="112" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="B112">
         <v>25.700000760000002</v>
@@ -4378,9 +4378,9 @@
         <v>0.39</v>
       </c>
     </row>
-    <row r="113" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="B113">
         <v>25.799999239999998</v>
@@ -4407,9 +4407,9 @@
         <v>-1.72</v>
       </c>
     </row>
-    <row r="114" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="B114">
         <v>26.299999239999998</v>
@@ -4436,9 +4436,9 @@
         <v>-0.56999999999999995</v>
       </c>
     </row>
-    <row r="115" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="B115">
         <v>26.25</v>
@@ -4465,9 +4465,9 @@
         <v>0.19</v>
       </c>
     </row>
-    <row r="116" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="B116">
         <v>26.399999619999999</v>
@@ -4494,9 +4494,9 @@
         <v>-0.56999999999999995</v>
       </c>
     </row>
-    <row r="117" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="B117">
         <v>26.100000380000001</v>
@@ -4523,9 +4523,9 @@
         <v>1.1499999999999999</v>
       </c>
     </row>
-    <row r="118" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="B118">
         <v>25.899999619999999</v>
@@ -4552,9 +4552,9 @@
         <v>1.1599999999999999</v>
       </c>
     </row>
-    <row r="119" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="B119">
         <v>25.549999239999998</v>
@@ -4581,9 +4581,9 @@
         <v>1.18</v>
       </c>
     </row>
-    <row r="120" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="B120">
         <v>24.979999540000001</v>
@@ -4610,9 +4610,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="121" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="B121">
         <v>25.049999239999998</v>
@@ -4639,9 +4639,9 @@
         <v>-0.2</v>
       </c>
     </row>
-    <row r="122" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="B122">
         <v>24.5</v>
@@ -4668,9 +4668,9 @@
         <v>2.08</v>
       </c>
     </row>
-    <row r="123" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="B123">
         <v>24.5</v>
@@ -4697,9 +4697,9 @@
         <v>0.16</v>
       </c>
     </row>
-    <row r="124" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="B124">
         <v>24.340000150000002</v>
@@ -4726,9 +4726,9 @@
         <v>0.56999999999999995</v>
       </c>
     </row>
-    <row r="125" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="B125">
         <v>24.399999619999999</v>
@@ -4755,9 +4755,9 @@
         <v>-0.33</v>
       </c>
     </row>
-    <row r="126" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="B126">
         <v>24.579999919999999</v>
@@ -4784,9 +4784,9 @@
         <v>-0.65</v>
       </c>
     </row>
-    <row r="127" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="B127">
         <v>24.63999939</v>
@@ -4813,9 +4813,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="128" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="B128">
         <v>24.5</v>
@@ -4842,9 +4842,9 @@
         <v>0.99</v>
       </c>
     </row>
-    <row r="129" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="B129">
         <v>24.299999239999998</v>
@@ -4871,9 +4871,9 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="130" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="B130">
         <v>24.299999239999998</v>
@@ -4900,9 +4900,9 @@
         <v>-0.08</v>
       </c>
     </row>
-    <row r="131" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="B131">
         <v>23.899999619999999</v>
@@ -4929,9 +4929,9 @@
         <v>1.67</v>
       </c>
     </row>
-    <row r="132" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="B132">
         <v>24</v>
@@ -4958,9 +4958,9 @@
         <v>-0.42</v>
       </c>
     </row>
-    <row r="133" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="B133">
         <v>24.260000229999999</v>
@@ -4987,9 +4987,9 @@
         <v>-1.1499999999999999</v>
       </c>
     </row>
-    <row r="134" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="B134">
         <v>24.299999239999998</v>
@@ -5016,9 +5016,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="135" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="B135">
         <v>24.700000760000002</v>
@@ -5045,9 +5045,9 @@
         <v>-1.3</v>
       </c>
     </row>
-    <row r="136" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="B136">
         <v>24.840000150000002</v>
@@ -5074,9 +5074,9 @@
         <v>-1.05</v>
       </c>
     </row>
-    <row r="137" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="B137">
         <v>24.799999239999998</v>
@@ -5103,9 +5103,9 @@
         <v>0.08</v>
       </c>
     </row>
-    <row r="138" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="B138">
         <v>24.780000690000001</v>
@@ -5132,9 +5132,9 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="139" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="B139">
         <v>25.149999619999999</v>
@@ -5161,9 +5161,9 @@
         <v>-2.21</v>
       </c>
     </row>
-    <row r="140" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="B140">
         <v>24.959999079999999</v>
@@ -5190,9 +5190,9 @@
         <v>1.36</v>
       </c>
     </row>
-    <row r="141" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="B141">
         <v>24.700000760000002</v>
@@ -5219,9 +5219,9 @@
         <v>1.22</v>
       </c>
     </row>
-    <row r="142" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="B142">
         <v>24.579999919999999</v>
@@ -5248,9 +5248,9 @@
         <v>0.49</v>
       </c>
     </row>
-    <row r="143" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="B143">
         <v>24.200000760000002</v>
@@ -5277,9 +5277,9 @@
         <v>1.83</v>
       </c>
     </row>
-    <row r="144" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="B144">
         <v>23.799999239999998</v>
@@ -5306,9 +5306,9 @@
         <v>0.92</v>
       </c>
     </row>
-    <row r="145" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="B145">
         <v>24</v>
@@ -5335,9 +5335,9 @@
         <v>-0.5</v>
       </c>
     </row>
-    <row r="146" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="B146">
         <v>24.100000380000001</v>
@@ -5364,9 +5364,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="147" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="B147">
         <v>24.120000839999999</v>
@@ -5393,9 +5393,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="148" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="B148">
         <v>24.959999079999999</v>
@@ -5422,9 +5422,9 @@
         <v>-3.61</v>
       </c>
     </row>
-    <row r="149" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="B149">
         <v>25.149999619999999</v>
@@ -5451,9 +5451,9 @@
         <v>-0.6</v>
       </c>
     </row>
-    <row r="150" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="B150">
         <v>25.299999239999998</v>
@@ -5480,9 +5480,9 @@
         <v>-0.6</v>
       </c>
     </row>
-    <row r="151" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="B151">
         <v>24.959999079999999</v>
@@ -5509,9 +5509,9 @@
         <v>1.86</v>
       </c>
     </row>
-    <row r="152" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="B152">
         <v>24.920000080000001</v>
@@ -5538,9 +5538,9 @@
         <v>-0.88</v>
       </c>
     </row>
-    <row r="153" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="B153">
         <v>25.25</v>
@@ -5567,9 +5567,9 @@
         <v>-1.1499999999999999</v>
       </c>
     </row>
-    <row r="154" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="B154">
         <v>25</v>
@@ -5596,9 +5596,9 @@
         <v>1.32</v>
       </c>
     </row>
-    <row r="155" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="B155">
         <v>24.540000920000001</v>
@@ -5625,9 +5625,9 @@
         <v>2.5499999999999998</v>
       </c>
     </row>
-    <row r="156" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="B156">
         <v>24.299999239999998</v>
@@ -5654,9 +5654,9 @@
         <v>-0.33</v>
       </c>
     </row>
-    <row r="157" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="B157">
         <v>25.100000380000001</v>
@@ -5683,9 +5683,9 @@
         <v>-3.83</v>
       </c>
     </row>
-    <row r="158" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A158" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="B158">
         <v>25.5</v>
@@ -5712,9 +5712,9 @@
         <v>-1.74</v>
       </c>
     </row>
-    <row r="159" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A159" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="B159">
         <v>25.799999239999998</v>
@@ -5741,9 +5741,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="160" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A160" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="B160">
         <v>25.600000380000001</v>
@@ -5770,9 +5770,9 @@
         <v>0.78</v>
       </c>
     </row>
-    <row r="161" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A161" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="B161">
         <v>26</v>
@@ -5799,9 +5799,9 @@
         <v>-1.54</v>
       </c>
     </row>
-    <row r="162" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A162" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="B162">
         <v>26.299999239999998</v>
@@ -5828,9 +5828,9 @@
         <v>-2.0699999999999998</v>
       </c>
     </row>
-    <row r="163" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A163" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="B163">
         <v>27</v>
@@ -5857,9 +5857,9 @@
         <v>-1.67</v>
       </c>
     </row>
-    <row r="164" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A164" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="B164">
         <v>26.950000760000002</v>
@@ -5886,9 +5886,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="165" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A165" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="B165">
         <v>27</v>
@@ -5915,9 +5915,9 @@
         <v>-0.37</v>
       </c>
     </row>
-    <row r="166" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A166" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="B166">
         <v>26.850000380000001</v>
@@ -5944,9 +5944,9 @@
         <v>0.93</v>
       </c>
     </row>
-    <row r="167" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A167" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="B167">
         <v>27.299999239999998</v>
@@ -5973,9 +5973,9 @@
         <v>-1.65</v>
       </c>
     </row>
-    <row r="168" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A168" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="B168">
         <v>27.549999239999998</v>
@@ -6002,9 +6002,9 @@
         <v>-1.0900000000000001</v>
       </c>
     </row>
-    <row r="169" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A169" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="B169">
         <v>27.75</v>
@@ -6031,9 +6031,9 @@
         <v>-0.54</v>
       </c>
     </row>
-    <row r="170" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A170" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="B170">
         <v>27.75</v>
@@ -6060,9 +6060,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="171" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A171" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="B171">
         <v>27.649999619999999</v>
@@ -6089,9 +6089,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="172" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A172" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="B172">
         <v>28.049999239999998</v>
@@ -6118,9 +6118,9 @@
         <v>-0.89</v>
       </c>
     </row>
-    <row r="173" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A173" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B173">
         <v>26.799999239999998</v>
@@ -6147,9 +6147,9 @@
         <v>5.26</v>
       </c>
     </row>
-    <row r="174" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A174" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="B174">
         <v>26.950000760000002</v>
@@ -6176,9 +6176,9 @@
         <v>-0.93</v>
       </c>
     </row>
-    <row r="175" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A175" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="B175">
         <v>25.799999239999998</v>
@@ -6205,9 +6205,9 @@
         <v>4.07</v>
       </c>
     </row>
-    <row r="176" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A176" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="B176">
         <v>25.049999239999998</v>
@@ -6234,9 +6234,9 @@
         <v>2.99</v>
       </c>
     </row>
-    <row r="177" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A177" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="B177">
         <v>24.940000529999999</v>
@@ -6263,9 +6263,9 @@
         <v>0.44</v>
       </c>
     </row>
-    <row r="178" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A178" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="B178">
         <v>25.049999239999998</v>
@@ -6292,9 +6292,9 @@
         <v>-0.64</v>
       </c>
     </row>
-    <row r="179" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A179" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="B179">
         <v>25</v>
@@ -6321,9 +6321,9 @@
         <v>0.56000000000000005</v>
       </c>
     </row>
-    <row r="180" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A180" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="B180">
         <v>24.780000690000001</v>
@@ -6350,9 +6350,9 @@
         <v>0.73</v>
       </c>
     </row>
-    <row r="181" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A181" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="B181">
         <v>24.719999309999999</v>
@@ -6379,9 +6379,9 @@
         <v>0.24</v>
       </c>
     </row>
-    <row r="182" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A182" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="B182">
         <v>24.68000031</v>
@@ -6408,9 +6408,9 @@
         <v>-0.08</v>
       </c>
     </row>
-    <row r="183" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A183" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="B183">
         <v>24.620000839999999</v>
@@ -6437,9 +6437,9 @@
         <v>0.49</v>
       </c>
     </row>
-    <row r="184" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A184" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="B184">
         <v>24.5</v>
@@ -6466,9 +6466,9 @@
         <v>0.49</v>
       </c>
     </row>
-    <row r="185" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A185" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="B185">
         <v>24.459999079999999</v>
@@ -6495,9 +6495,9 @@
         <v>0.08</v>
       </c>
     </row>
-    <row r="186" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A186" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="B186">
         <v>24.299999239999998</v>
@@ -6524,9 +6524,9 @@
         <v>0.82</v>
       </c>
     </row>
-    <row r="187" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A187" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="B187">
         <v>24.239999770000001</v>
@@ -6553,9 +6553,9 @@
         <v>0.08</v>
       </c>
     </row>
-    <row r="188" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A188" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="B188">
         <v>24.200000760000002</v>
@@ -6582,9 +6582,9 @@
         <v>0.17</v>
       </c>
     </row>
-    <row r="189" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A189" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="B189">
         <v>24.260000229999999</v>
@@ -6611,9 +6611,9 @@
         <v>-0.16</v>
       </c>
     </row>
-    <row r="190" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A190" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="B190">
         <v>24.13999939</v>
@@ -6640,9 +6640,9 @@
         <v>-2.88</v>
       </c>
     </row>
-    <row r="191" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A191" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="B191">
         <v>24.959999079999999</v>
@@ -6669,9 +6669,9 @@
         <v>0.16</v>
       </c>
     </row>
-    <row r="192" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A192" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="B192">
         <v>25</v>
@@ -6698,9 +6698,9 @@
         <v>-0.24</v>
       </c>
     </row>
-    <row r="193" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A193" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="B193">
         <v>24.899999619999999</v>
@@ -6727,9 +6727,9 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="194" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A194" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="B194">
         <v>24.420000080000001</v>
@@ -6756,9 +6756,9 @@
         <v>1.97</v>
       </c>
     </row>
-    <row r="195" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A195" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="B195">
         <v>24.459999079999999</v>
@@ -6785,9 +6785,9 @@
         <v>-0.25</v>
       </c>
     </row>
-    <row r="196" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A196" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="B196">
         <v>24.440000529999999</v>
@@ -6814,9 +6814,9 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="197" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A197" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="B197">
         <v>24.31999969</v>
@@ -6843,9 +6843,9 @@
         <v>0.08</v>
       </c>
     </row>
-    <row r="198" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A198" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="B198">
         <v>24.399999619999999</v>
@@ -6872,9 +6872,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="199" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A199" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="B199">
         <v>24.260000229999999</v>
@@ -6901,9 +6901,9 @@
         <v>0.74</v>
       </c>
     </row>
-    <row r="200" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A200" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="B200">
         <v>24.200000760000002</v>
@@ -6930,9 +6930,9 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="201" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A201" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="B201">
         <v>24.100000380000001</v>
@@ -6959,9 +6959,9 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="202" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A202" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="B202">
         <v>24.120000839999999</v>
@@ -6988,9 +6988,9 @@
         <v>-0.25</v>
       </c>
     </row>
-    <row r="203" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A203" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="B203">
         <v>24.159999849999998</v>
@@ -7017,9 +7017,9 @@
         <v>0.17</v>
       </c>
     </row>
-    <row r="204" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A204" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="B204">
         <v>24.31999969</v>
@@ -7046,9 +7046,9 @@
         <v>-1.23</v>
       </c>
     </row>
-    <row r="205" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A205" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="B205">
         <v>24.299999239999998</v>
@@ -7075,9 +7075,9 @@
         <v>0.41</v>
       </c>
     </row>
-    <row r="206" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A206" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="B206">
         <v>24.299999239999998</v>
@@ -7104,9 +7104,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="207" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A207" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="B207">
         <v>24.239999770000001</v>
@@ -7133,9 +7133,9 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="208" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A208" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="B208">
         <v>24.100000380000001</v>
@@ -7162,9 +7162,9 @@
         <v>0.41</v>
       </c>
     </row>
-    <row r="209" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A209" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="B209">
         <v>23.959999079999999</v>
@@ -7191,9 +7191,9 @@
         <v>0.57999999999999996</v>
       </c>
     </row>
-    <row r="210" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A210" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="B210">
         <v>24.040000920000001</v>
@@ -7220,9 +7220,9 @@
         <v>-0.08</v>
       </c>
     </row>
-    <row r="211" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A211" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="B211">
         <v>23.920000080000001</v>
@@ -7249,9 +7249,9 @@
         <v>0.42</v>
       </c>
     </row>
-    <row r="212" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A212" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="B212">
         <v>23.959999079999999</v>
@@ -7278,9 +7278,9 @@
         <v>-0.42</v>
       </c>
     </row>
-    <row r="213" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A213" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="B213">
         <v>24.040000920000001</v>
@@ -7307,9 +7307,9 @@
         <v>-0.25</v>
       </c>
     </row>
-    <row r="214" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A214" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="B214">
         <v>24.020000459999999</v>
@@ -7336,9 +7336,9 @@
         <v>0.17</v>
       </c>
     </row>
-    <row r="215" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A215" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="B215">
         <v>24</v>
@@ -7365,9 +7365,9 @@
         <v>0.08</v>
       </c>
     </row>
-    <row r="216" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A216" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="B216">
         <v>24</v>
@@ -7394,9 +7394,9 @@
         <v>0.08</v>
       </c>
     </row>
-    <row r="217" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A217" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="B217">
         <v>24</v>
@@ -7423,9 +7423,9 @@
         <v>-0.08</v>
       </c>
     </row>
-    <row r="218" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A218" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="B218">
         <v>24.100000380000001</v>
@@ -7452,9 +7452,9 @@
         <v>-0.25</v>
       </c>
     </row>
-    <row r="219" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A219" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="B219">
         <v>24</v>
@@ -7481,9 +7481,9 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="220" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A220" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="B220">
         <v>24.020000459999999</v>
@@ -7510,9 +7510,9 @@
         <v>-0.25</v>
       </c>
     </row>
-    <row r="221" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A221" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="B221">
         <v>24</v>
@@ -7539,9 +7539,9 @@
         <v>0.17</v>
       </c>
     </row>
-    <row r="222" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A222" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="B222">
         <v>24.079999919999999</v>
@@ -7568,9 +7568,9 @@
         <v>-0.17</v>
       </c>
     </row>
-    <row r="223" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A223" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="B223">
         <v>24.13999939</v>
@@ -7597,9 +7597,9 @@
         <v>-0.33</v>
       </c>
     </row>
-    <row r="224" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A224" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="B224">
         <v>24.260000229999999</v>
@@ -7626,9 +7626,9 @@
         <v>-0.33</v>
       </c>
     </row>
-    <row r="225" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A225" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="B225">
         <v>24.280000690000001</v>
@@ -7655,9 +7655,9 @@
         <v>-0.25</v>
       </c>
     </row>
-    <row r="226" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A226" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="B226">
         <v>24.159999849999998</v>
@@ -7684,9 +7684,9 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="227" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A227" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="B227">
         <v>24.219999309999999</v>
@@ -7713,9 +7713,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="228" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A228" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="B228">
         <v>24.18000031</v>
@@ -7742,9 +7742,9 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="229" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A229" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="B229">
         <v>24.399999619999999</v>
@@ -7771,9 +7771,9 @@
         <v>-1.07</v>
       </c>
     </row>
-    <row r="230" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A230" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="B230">
         <v>24.579999919999999</v>
@@ -7800,9 +7800,9 @@
         <v>-0.73</v>
       </c>
     </row>
-    <row r="231" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A231" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="B231">
         <v>24.579999919999999</v>
@@ -7829,9 +7829,9 @@
         <v>0.08</v>
       </c>
     </row>
-    <row r="232" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A232" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="B232">
         <v>24.260000229999999</v>
@@ -7858,9 +7858,9 @@
         <v>1.1499999999999999</v>
       </c>
     </row>
-    <row r="233" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A233" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="B233">
         <v>23.920000080000001</v>
@@ -7887,9 +7887,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="234" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A234" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="B234">
         <v>24.100000380000001</v>
@@ -7916,9 +7916,9 @@
         <v>-0.25</v>
       </c>
     </row>
-    <row r="235" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A235" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="B235">
         <v>24</v>
@@ -7945,9 +7945,9 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="236" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A236" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="B236">
         <v>24</v>
@@ -7974,9 +7974,9 @@
         <v>0.08</v>
       </c>
     </row>
-    <row r="237" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A237" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="B237">
         <v>23.840000150000002</v>
@@ -8003,9 +8003,9 @@
         <v>0.59</v>
       </c>
     </row>
-    <row r="238" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A238" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="B238">
         <v>24.020000459999999</v>
@@ -8032,9 +8032,9 @@
         <v>-0.67</v>
       </c>
     </row>
-    <row r="239" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A239" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="B239">
         <v>24</v>
@@ -8061,9 +8061,9 @@
         <v>0.08</v>
       </c>
     </row>
-    <row r="240" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A240" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="B240">
         <v>24.079999919999999</v>
@@ -8090,9 +8090,9 @@
         <v>-0.25</v>
       </c>
     </row>
-    <row r="241" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A241" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="B241">
         <v>24</v>
@@ -8119,9 +8119,9 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="242" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A242" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="B242">
         <v>24.020000459999999</v>
@@ -8148,9 +8148,9 @@
         <v>-0.33</v>
       </c>
     </row>
-    <row r="243" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A243" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="B243">
         <v>24</v>
@@ -8177,9 +8177,9 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="244" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A244" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="B244">
         <v>23.879999160000001</v>
@@ -8206,9 +8206,9 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="245" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A245" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="B245">
         <v>23.879999160000001</v>
@@ -8235,9 +8235,9 @@
         <v>0.34</v>
       </c>
     </row>
-    <row r="246" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A246" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="B246">
         <v>23.840000150000002</v>
@@ -8264,9 +8264,9 @@
         <v>0.17</v>
       </c>
     </row>
-    <row r="247" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A247" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="B247">
         <v>23.600000380000001</v>
@@ -8293,9 +8293,9 @@
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="248" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A248" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="B248">
         <v>23.479999540000001</v>
@@ -8322,9 +8322,9 @@
         <v>0.68</v>
       </c>
     </row>
-    <row r="249" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A249" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="B249">
         <v>23.059999470000001</v>
@@ -8351,9 +8351,9 @@
         <v>1.56</v>
       </c>
     </row>
-    <row r="250" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A250" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="B250">
         <v>23.13999939</v>
@@ -8380,9 +8380,9 @@
         <v>-0.43</v>
       </c>
     </row>
-    <row r="251" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A251" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="B251">
         <v>22.979999540000001</v>
@@ -8411,5 +8411,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added Spearman and Pearson Correlation Functions
</commit_message>
<xml_diff>
--- a/1150.xlsx
+++ b/1150.xlsx
@@ -38,9 +38,6 @@
     <t xml:space="preserve"> Volume</t>
   </si>
   <si>
-    <t xml:space="preserve"> Turnover</t>
-  </si>
-  <si>
     <t xml:space="preserve"> 31/12/2019 </t>
   </si>
   <si>
@@ -801,6 +798,9 @@
   </si>
   <si>
     <t>Open</t>
+  </si>
+  <si>
+    <t>Turnover</t>
   </si>
 </sst>
 </file>
@@ -1118,10 +1118,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I251"/>
+  <dimension ref="A1:J251"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O15" sqref="O15"/>
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1130,12 +1130,12 @@
     <col min="7" max="7" width="26" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -1144,24 +1144,24 @@
         <v>2</v>
       </c>
       <c r="E1" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="F1" t="s">
         <v>3</v>
       </c>
       <c r="G1" t="s">
+        <v>258</v>
+      </c>
+      <c r="H1" t="s">
+        <v>255</v>
+      </c>
+      <c r="I1" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
         <v>4</v>
-      </c>
-      <c r="H1" t="s">
-        <v>256</v>
-      </c>
-      <c r="I1" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>5</v>
       </c>
       <c r="B2">
         <v>24.879999160000001</v>
@@ -1187,10 +1187,14 @@
       <c r="I2">
         <v>1.89</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J2">
+        <f>(I2-MIN(I2:I251))/(MAX(I2:I251)-MIN(I2:I251))</f>
+        <v>0.56315289648622968</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B3">
         <v>25.350000380000001</v>
@@ -1217,9 +1221,9 @@
         <v>-2.0499999999999998</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B4">
         <v>25.700000760000002</v>
@@ -1246,9 +1250,9 @@
         <v>-1.17</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B5">
         <v>25.799999239999998</v>
@@ -1275,9 +1279,9 @@
         <v>-0.39</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B6">
         <v>25.799999239999998</v>
@@ -1304,9 +1308,9 @@
         <v>-0.19</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B7">
         <v>25.899999619999999</v>
@@ -1333,9 +1337,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B8">
         <v>25.799999239999998</v>
@@ -1362,9 +1366,9 @@
         <v>0.19</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B9">
         <v>25.899999619999999</v>
@@ -1391,9 +1395,9 @@
         <v>-0.57999999999999996</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B10">
         <v>26.100000380000001</v>
@@ -1420,9 +1424,9 @@
         <v>-0.56999999999999995</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B11">
         <v>25.899999619999999</v>
@@ -1449,9 +1453,9 @@
         <v>0.38</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B12">
         <v>26.049999239999998</v>
@@ -1478,9 +1482,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B13">
         <v>25.799999239999998</v>
@@ -1507,9 +1511,9 @@
         <v>1.56</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B14">
         <v>25.049999239999998</v>
@@ -1536,9 +1540,9 @@
         <v>6.49</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B15">
         <v>24.36000061</v>
@@ -1565,9 +1569,9 @@
         <v>-1.31</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B16">
         <v>24</v>
@@ -1596,7 +1600,7 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B17">
         <v>24.059999470000001</v>
@@ -1625,7 +1629,7 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B18">
         <v>24.100000380000001</v>
@@ -1654,7 +1658,7 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B19">
         <v>23.079999919999999</v>
@@ -1683,7 +1687,7 @@
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B20">
         <v>23</v>
@@ -1712,7 +1716,7 @@
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B21">
         <v>23.100000380000001</v>
@@ -1741,7 +1745,7 @@
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B22">
         <v>22.879999160000001</v>
@@ -1770,7 +1774,7 @@
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B23">
         <v>22.979999540000001</v>
@@ -1799,7 +1803,7 @@
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B24">
         <v>22.86000061</v>
@@ -1828,7 +1832,7 @@
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B25">
         <v>22.600000380000001</v>
@@ -1857,7 +1861,7 @@
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B26">
         <v>22.81999969</v>
@@ -1886,7 +1890,7 @@
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B27">
         <v>22.86000061</v>
@@ -1915,7 +1919,7 @@
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B28">
         <v>22.760000229999999</v>
@@ -1944,7 +1948,7 @@
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B29">
         <v>23</v>
@@ -1973,7 +1977,7 @@
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B30">
         <v>22.879999160000001</v>
@@ -2002,7 +2006,7 @@
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B31">
         <v>22.879999160000001</v>
@@ -2031,7 +2035,7 @@
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B32">
         <v>22.659999849999998</v>
@@ -2060,7 +2064,7 @@
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B33">
         <v>22.299999239999998</v>
@@ -2089,7 +2093,7 @@
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B34">
         <v>22.059999470000001</v>
@@ -2118,7 +2122,7 @@
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B35">
         <v>22.059999470000001</v>
@@ -2147,7 +2151,7 @@
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B36">
         <v>22</v>
@@ -2176,7 +2180,7 @@
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B37">
         <v>21.86000061</v>
@@ -2205,7 +2209,7 @@
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B38">
         <v>21.799999239999998</v>
@@ -2234,7 +2238,7 @@
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B39">
         <v>21.200000760000002</v>
@@ -2263,7 +2267,7 @@
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B40">
         <v>20.86000061</v>
@@ -2292,7 +2296,7 @@
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B41">
         <v>21.200000760000002</v>
@@ -2321,7 +2325,7 @@
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B42">
         <v>21.13999939</v>
@@ -2350,7 +2354,7 @@
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B43">
         <v>20.899999619999999</v>
@@ -2379,7 +2383,7 @@
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B44">
         <v>20.700000760000002</v>
@@ -2408,7 +2412,7 @@
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B45">
         <v>21.13999939</v>
@@ -2437,7 +2441,7 @@
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B46">
         <v>20.63999939</v>
@@ -2466,7 +2470,7 @@
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B47">
         <v>21.020000459999999</v>
@@ -2495,7 +2499,7 @@
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B48">
         <v>21.459999079999999</v>
@@ -2524,7 +2528,7 @@
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B49">
         <v>21.68000031</v>
@@ -2553,7 +2557,7 @@
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B50">
         <v>21.799999239999998</v>
@@ -2582,7 +2586,7 @@
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B51">
         <v>21.520000459999999</v>
@@ -2611,7 +2615,7 @@
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B52">
         <v>20.840000150000002</v>
@@ -2640,7 +2644,7 @@
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B53">
         <v>20.799999239999998</v>
@@ -2669,7 +2673,7 @@
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B54">
         <v>20.5</v>
@@ -2698,7 +2702,7 @@
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B55">
         <v>20.100000380000001</v>
@@ -2727,7 +2731,7 @@
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B56">
         <v>19.700000760000002</v>
@@ -2756,7 +2760,7 @@
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B57">
         <v>20.040000920000001</v>
@@ -2785,7 +2789,7 @@
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B58">
         <v>20.340000150000002</v>
@@ -2814,7 +2818,7 @@
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B59">
         <v>20.479999540000001</v>
@@ -2843,7 +2847,7 @@
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B60">
         <v>20.600000380000001</v>
@@ -2872,7 +2876,7 @@
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B61">
         <v>21.260000229999999</v>
@@ -2901,7 +2905,7 @@
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B62">
         <v>21.5</v>
@@ -2930,7 +2934,7 @@
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B63">
         <v>21.81999969</v>
@@ -2959,7 +2963,7 @@
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B64">
         <v>22.020000459999999</v>
@@ -2988,7 +2992,7 @@
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B65">
         <v>21.899999619999999</v>
@@ -3017,7 +3021,7 @@
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B66">
         <v>22.200000760000002</v>
@@ -3046,7 +3050,7 @@
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B67">
         <v>22.600000380000001</v>
@@ -3075,7 +3079,7 @@
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B68">
         <v>22.36000061</v>
@@ -3104,7 +3108,7 @@
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B69">
         <v>22.079999919999999</v>
@@ -3133,7 +3137,7 @@
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B70">
         <v>22.020000459999999</v>
@@ -3162,7 +3166,7 @@
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B71">
         <v>22.200000760000002</v>
@@ -3191,7 +3195,7 @@
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B72">
         <v>21.920000080000001</v>
@@ -3220,7 +3224,7 @@
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B73">
         <v>21.879999160000001</v>
@@ -3249,7 +3253,7 @@
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B74">
         <v>21.420000080000001</v>
@@ -3278,7 +3282,7 @@
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B75">
         <v>21.799999239999998</v>
@@ -3307,7 +3311,7 @@
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B76">
         <v>21.600000380000001</v>
@@ -3336,7 +3340,7 @@
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B77">
         <v>21.440000529999999</v>
@@ -3365,7 +3369,7 @@
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B78">
         <v>20.899999619999999</v>
@@ -3394,7 +3398,7 @@
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B79">
         <v>21.18000031</v>
@@ -3423,7 +3427,7 @@
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B80">
         <v>21.780000690000001</v>
@@ -3452,7 +3456,7 @@
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B81">
         <v>22.079999919999999</v>
@@ -3481,7 +3485,7 @@
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B82">
         <v>22.100000380000001</v>
@@ -3510,7 +3514,7 @@
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B83">
         <v>22.120000839999999</v>
@@ -3539,7 +3543,7 @@
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B84">
         <v>22.219999309999999</v>
@@ -3568,7 +3572,7 @@
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B85">
         <v>21.940000529999999</v>
@@ -3597,7 +3601,7 @@
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B86">
         <v>22.059999470000001</v>
@@ -3626,7 +3630,7 @@
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B87">
         <v>21.81999969</v>
@@ -3655,7 +3659,7 @@
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B88">
         <v>22</v>
@@ -3684,7 +3688,7 @@
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B89">
         <v>22.31999969</v>
@@ -3713,7 +3717,7 @@
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B90">
         <v>22.5</v>
@@ -3742,7 +3746,7 @@
     </row>
     <row r="91" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B91">
         <v>23.219999309999999</v>
@@ -3771,7 +3775,7 @@
     </row>
     <row r="92" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B92">
         <v>22.840000150000002</v>
@@ -3800,7 +3804,7 @@
     </row>
     <row r="93" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B93">
         <v>23.600000380000001</v>
@@ -3829,7 +3833,7 @@
     </row>
     <row r="94" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B94">
         <v>23.920000080000001</v>
@@ -3858,7 +3862,7 @@
     </row>
     <row r="95" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B95">
         <v>24.100000380000001</v>
@@ -3887,7 +3891,7 @@
     </row>
     <row r="96" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B96">
         <v>24.219999309999999</v>
@@ -3916,7 +3920,7 @@
     </row>
     <row r="97" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B97">
         <v>24.100000380000001</v>
@@ -3945,7 +3949,7 @@
     </row>
     <row r="98" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B98">
         <v>24.13999939</v>
@@ -3974,7 +3978,7 @@
     </row>
     <row r="99" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B99">
         <v>24.36000061</v>
@@ -4003,7 +4007,7 @@
     </row>
     <row r="100" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B100">
         <v>24.399999619999999</v>
@@ -4032,7 +4036,7 @@
     </row>
     <row r="101" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B101">
         <v>24.159999849999998</v>
@@ -4061,7 +4065,7 @@
     </row>
     <row r="102" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B102">
         <v>24.879999160000001</v>
@@ -4090,7 +4094,7 @@
     </row>
     <row r="103" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B103">
         <v>24.600000380000001</v>
@@ -4119,7 +4123,7 @@
     </row>
     <row r="104" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B104">
         <v>24.879999160000001</v>
@@ -4148,7 +4152,7 @@
     </row>
     <row r="105" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B105">
         <v>24.879999160000001</v>
@@ -4177,7 +4181,7 @@
     </row>
     <row r="106" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B106">
         <v>25</v>
@@ -4206,7 +4210,7 @@
     </row>
     <row r="107" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B107">
         <v>25.549999239999998</v>
@@ -4235,7 +4239,7 @@
     </row>
     <row r="108" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B108">
         <v>25.450000760000002</v>
@@ -4264,7 +4268,7 @@
     </row>
     <row r="109" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B109">
         <v>25.350000380000001</v>
@@ -4293,7 +4297,7 @@
     </row>
     <row r="110" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B110">
         <v>25.299999239999998</v>
@@ -4322,7 +4326,7 @@
     </row>
     <row r="111" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B111">
         <v>25.700000760000002</v>
@@ -4351,7 +4355,7 @@
     </row>
     <row r="112" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B112">
         <v>25.700000760000002</v>
@@ -4380,7 +4384,7 @@
     </row>
     <row r="113" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B113">
         <v>25.799999239999998</v>
@@ -4409,7 +4413,7 @@
     </row>
     <row r="114" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B114">
         <v>26.299999239999998</v>
@@ -4438,7 +4442,7 @@
     </row>
     <row r="115" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B115">
         <v>26.25</v>
@@ -4467,7 +4471,7 @@
     </row>
     <row r="116" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B116">
         <v>26.399999619999999</v>
@@ -4496,7 +4500,7 @@
     </row>
     <row r="117" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B117">
         <v>26.100000380000001</v>
@@ -4525,7 +4529,7 @@
     </row>
     <row r="118" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B118">
         <v>25.899999619999999</v>
@@ -4554,7 +4558,7 @@
     </row>
     <row r="119" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B119">
         <v>25.549999239999998</v>
@@ -4583,7 +4587,7 @@
     </row>
     <row r="120" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B120">
         <v>24.979999540000001</v>
@@ -4612,7 +4616,7 @@
     </row>
     <row r="121" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B121">
         <v>25.049999239999998</v>
@@ -4641,7 +4645,7 @@
     </row>
     <row r="122" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B122">
         <v>24.5</v>
@@ -4670,7 +4674,7 @@
     </row>
     <row r="123" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B123">
         <v>24.5</v>
@@ -4699,7 +4703,7 @@
     </row>
     <row r="124" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B124">
         <v>24.340000150000002</v>
@@ -4728,7 +4732,7 @@
     </row>
     <row r="125" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B125">
         <v>24.399999619999999</v>
@@ -4757,7 +4761,7 @@
     </row>
     <row r="126" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B126">
         <v>24.579999919999999</v>
@@ -4786,7 +4790,7 @@
     </row>
     <row r="127" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B127">
         <v>24.63999939</v>
@@ -4815,7 +4819,7 @@
     </row>
     <row r="128" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B128">
         <v>24.5</v>
@@ -4844,7 +4848,7 @@
     </row>
     <row r="129" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B129">
         <v>24.299999239999998</v>
@@ -4873,7 +4877,7 @@
     </row>
     <row r="130" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B130">
         <v>24.299999239999998</v>
@@ -4902,7 +4906,7 @@
     </row>
     <row r="131" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B131">
         <v>23.899999619999999</v>
@@ -4931,7 +4935,7 @@
     </row>
     <row r="132" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B132">
         <v>24</v>
@@ -4960,7 +4964,7 @@
     </row>
     <row r="133" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B133">
         <v>24.260000229999999</v>
@@ -4989,7 +4993,7 @@
     </row>
     <row r="134" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B134">
         <v>24.299999239999998</v>
@@ -5018,7 +5022,7 @@
     </row>
     <row r="135" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B135">
         <v>24.700000760000002</v>
@@ -5047,7 +5051,7 @@
     </row>
     <row r="136" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B136">
         <v>24.840000150000002</v>
@@ -5076,7 +5080,7 @@
     </row>
     <row r="137" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B137">
         <v>24.799999239999998</v>
@@ -5105,7 +5109,7 @@
     </row>
     <row r="138" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B138">
         <v>24.780000690000001</v>
@@ -5134,7 +5138,7 @@
     </row>
     <row r="139" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B139">
         <v>25.149999619999999</v>
@@ -5163,7 +5167,7 @@
     </row>
     <row r="140" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B140">
         <v>24.959999079999999</v>
@@ -5192,7 +5196,7 @@
     </row>
     <row r="141" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B141">
         <v>24.700000760000002</v>
@@ -5221,7 +5225,7 @@
     </row>
     <row r="142" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B142">
         <v>24.579999919999999</v>
@@ -5250,7 +5254,7 @@
     </row>
     <row r="143" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B143">
         <v>24.200000760000002</v>
@@ -5279,7 +5283,7 @@
     </row>
     <row r="144" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B144">
         <v>23.799999239999998</v>
@@ -5308,7 +5312,7 @@
     </row>
     <row r="145" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B145">
         <v>24</v>
@@ -5337,7 +5341,7 @@
     </row>
     <row r="146" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B146">
         <v>24.100000380000001</v>
@@ -5366,7 +5370,7 @@
     </row>
     <row r="147" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B147">
         <v>24.120000839999999</v>
@@ -5395,7 +5399,7 @@
     </row>
     <row r="148" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B148">
         <v>24.959999079999999</v>
@@ -5424,7 +5428,7 @@
     </row>
     <row r="149" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B149">
         <v>25.149999619999999</v>
@@ -5453,7 +5457,7 @@
     </row>
     <row r="150" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B150">
         <v>25.299999239999998</v>
@@ -5482,7 +5486,7 @@
     </row>
     <row r="151" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B151">
         <v>24.959999079999999</v>
@@ -5511,7 +5515,7 @@
     </row>
     <row r="152" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B152">
         <v>24.920000080000001</v>
@@ -5540,7 +5544,7 @@
     </row>
     <row r="153" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B153">
         <v>25.25</v>
@@ -5569,7 +5573,7 @@
     </row>
     <row r="154" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B154">
         <v>25</v>
@@ -5598,7 +5602,7 @@
     </row>
     <row r="155" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B155">
         <v>24.540000920000001</v>
@@ -5627,7 +5631,7 @@
     </row>
     <row r="156" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B156">
         <v>24.299999239999998</v>
@@ -5656,7 +5660,7 @@
     </row>
     <row r="157" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B157">
         <v>25.100000380000001</v>
@@ -5685,7 +5689,7 @@
     </row>
     <row r="158" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A158" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B158">
         <v>25.5</v>
@@ -5714,7 +5718,7 @@
     </row>
     <row r="159" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A159" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B159">
         <v>25.799999239999998</v>
@@ -5743,7 +5747,7 @@
     </row>
     <row r="160" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A160" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B160">
         <v>25.600000380000001</v>
@@ -5772,7 +5776,7 @@
     </row>
     <row r="161" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A161" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B161">
         <v>26</v>
@@ -5801,7 +5805,7 @@
     </row>
     <row r="162" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A162" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B162">
         <v>26.299999239999998</v>
@@ -5830,7 +5834,7 @@
     </row>
     <row r="163" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A163" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B163">
         <v>27</v>
@@ -5859,7 +5863,7 @@
     </row>
     <row r="164" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A164" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B164">
         <v>26.950000760000002</v>
@@ -5888,7 +5892,7 @@
     </row>
     <row r="165" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A165" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B165">
         <v>27</v>
@@ -5917,7 +5921,7 @@
     </row>
     <row r="166" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A166" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B166">
         <v>26.850000380000001</v>
@@ -5946,7 +5950,7 @@
     </row>
     <row r="167" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A167" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B167">
         <v>27.299999239999998</v>
@@ -5975,7 +5979,7 @@
     </row>
     <row r="168" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A168" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B168">
         <v>27.549999239999998</v>
@@ -6004,7 +6008,7 @@
     </row>
     <row r="169" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A169" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B169">
         <v>27.75</v>
@@ -6033,7 +6037,7 @@
     </row>
     <row r="170" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A170" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B170">
         <v>27.75</v>
@@ -6062,7 +6066,7 @@
     </row>
     <row r="171" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A171" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B171">
         <v>27.649999619999999</v>
@@ -6091,7 +6095,7 @@
     </row>
     <row r="172" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A172" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B172">
         <v>28.049999239999998</v>
@@ -6120,7 +6124,7 @@
     </row>
     <row r="173" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A173" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B173">
         <v>26.799999239999998</v>
@@ -6149,7 +6153,7 @@
     </row>
     <row r="174" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A174" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B174">
         <v>26.950000760000002</v>
@@ -6178,7 +6182,7 @@
     </row>
     <row r="175" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A175" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B175">
         <v>25.799999239999998</v>
@@ -6207,7 +6211,7 @@
     </row>
     <row r="176" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A176" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B176">
         <v>25.049999239999998</v>
@@ -6236,7 +6240,7 @@
     </row>
     <row r="177" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A177" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B177">
         <v>24.940000529999999</v>
@@ -6265,7 +6269,7 @@
     </row>
     <row r="178" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A178" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B178">
         <v>25.049999239999998</v>
@@ -6294,7 +6298,7 @@
     </row>
     <row r="179" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A179" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B179">
         <v>25</v>
@@ -6323,7 +6327,7 @@
     </row>
     <row r="180" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A180" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B180">
         <v>24.780000690000001</v>
@@ -6352,7 +6356,7 @@
     </row>
     <row r="181" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A181" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B181">
         <v>24.719999309999999</v>
@@ -6381,7 +6385,7 @@
     </row>
     <row r="182" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A182" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B182">
         <v>24.68000031</v>
@@ -6410,7 +6414,7 @@
     </row>
     <row r="183" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A183" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B183">
         <v>24.620000839999999</v>
@@ -6439,7 +6443,7 @@
     </row>
     <row r="184" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A184" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B184">
         <v>24.5</v>
@@ -6468,7 +6472,7 @@
     </row>
     <row r="185" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A185" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B185">
         <v>24.459999079999999</v>
@@ -6497,7 +6501,7 @@
     </row>
     <row r="186" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A186" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B186">
         <v>24.299999239999998</v>
@@ -6526,7 +6530,7 @@
     </row>
     <row r="187" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A187" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B187">
         <v>24.239999770000001</v>
@@ -6555,7 +6559,7 @@
     </row>
     <row r="188" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A188" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B188">
         <v>24.200000760000002</v>
@@ -6584,7 +6588,7 @@
     </row>
     <row r="189" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A189" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B189">
         <v>24.260000229999999</v>
@@ -6613,7 +6617,7 @@
     </row>
     <row r="190" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A190" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B190">
         <v>24.13999939</v>
@@ -6642,7 +6646,7 @@
     </row>
     <row r="191" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A191" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B191">
         <v>24.959999079999999</v>
@@ -6671,7 +6675,7 @@
     </row>
     <row r="192" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A192" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B192">
         <v>25</v>
@@ -6700,7 +6704,7 @@
     </row>
     <row r="193" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A193" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B193">
         <v>24.899999619999999</v>
@@ -6729,7 +6733,7 @@
     </row>
     <row r="194" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A194" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B194">
         <v>24.420000080000001</v>
@@ -6758,7 +6762,7 @@
     </row>
     <row r="195" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A195" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B195">
         <v>24.459999079999999</v>
@@ -6787,7 +6791,7 @@
     </row>
     <row r="196" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A196" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B196">
         <v>24.440000529999999</v>
@@ -6816,7 +6820,7 @@
     </row>
     <row r="197" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A197" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B197">
         <v>24.31999969</v>
@@ -6845,7 +6849,7 @@
     </row>
     <row r="198" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A198" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B198">
         <v>24.399999619999999</v>
@@ -6874,7 +6878,7 @@
     </row>
     <row r="199" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A199" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B199">
         <v>24.260000229999999</v>
@@ -6903,7 +6907,7 @@
     </row>
     <row r="200" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A200" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B200">
         <v>24.200000760000002</v>
@@ -6932,7 +6936,7 @@
     </row>
     <row r="201" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A201" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B201">
         <v>24.100000380000001</v>
@@ -6961,7 +6965,7 @@
     </row>
     <row r="202" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A202" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B202">
         <v>24.120000839999999</v>
@@ -6990,7 +6994,7 @@
     </row>
     <row r="203" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A203" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B203">
         <v>24.159999849999998</v>
@@ -7019,7 +7023,7 @@
     </row>
     <row r="204" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A204" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B204">
         <v>24.31999969</v>
@@ -7048,7 +7052,7 @@
     </row>
     <row r="205" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A205" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B205">
         <v>24.299999239999998</v>
@@ -7077,7 +7081,7 @@
     </row>
     <row r="206" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A206" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B206">
         <v>24.299999239999998</v>
@@ -7106,7 +7110,7 @@
     </row>
     <row r="207" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A207" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B207">
         <v>24.239999770000001</v>
@@ -7135,7 +7139,7 @@
     </row>
     <row r="208" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A208" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B208">
         <v>24.100000380000001</v>
@@ -7164,7 +7168,7 @@
     </row>
     <row r="209" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A209" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B209">
         <v>23.959999079999999</v>
@@ -7193,7 +7197,7 @@
     </row>
     <row r="210" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A210" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B210">
         <v>24.040000920000001</v>
@@ -7222,7 +7226,7 @@
     </row>
     <row r="211" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A211" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B211">
         <v>23.920000080000001</v>
@@ -7251,7 +7255,7 @@
     </row>
     <row r="212" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A212" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B212">
         <v>23.959999079999999</v>
@@ -7280,7 +7284,7 @@
     </row>
     <row r="213" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A213" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B213">
         <v>24.040000920000001</v>
@@ -7309,7 +7313,7 @@
     </row>
     <row r="214" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A214" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B214">
         <v>24.020000459999999</v>
@@ -7338,7 +7342,7 @@
     </row>
     <row r="215" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A215" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B215">
         <v>24</v>
@@ -7367,7 +7371,7 @@
     </row>
     <row r="216" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A216" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B216">
         <v>24</v>
@@ -7396,7 +7400,7 @@
     </row>
     <row r="217" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A217" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B217">
         <v>24</v>
@@ -7425,7 +7429,7 @@
     </row>
     <row r="218" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A218" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B218">
         <v>24.100000380000001</v>
@@ -7454,7 +7458,7 @@
     </row>
     <row r="219" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A219" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B219">
         <v>24</v>
@@ -7483,7 +7487,7 @@
     </row>
     <row r="220" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A220" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B220">
         <v>24.020000459999999</v>
@@ -7512,7 +7516,7 @@
     </row>
     <row r="221" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A221" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B221">
         <v>24</v>
@@ -7541,7 +7545,7 @@
     </row>
     <row r="222" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A222" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B222">
         <v>24.079999919999999</v>
@@ -7570,7 +7574,7 @@
     </row>
     <row r="223" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A223" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B223">
         <v>24.13999939</v>
@@ -7599,7 +7603,7 @@
     </row>
     <row r="224" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A224" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B224">
         <v>24.260000229999999</v>
@@ -7628,7 +7632,7 @@
     </row>
     <row r="225" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A225" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B225">
         <v>24.280000690000001</v>
@@ -7657,7 +7661,7 @@
     </row>
     <row r="226" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A226" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B226">
         <v>24.159999849999998</v>
@@ -7686,7 +7690,7 @@
     </row>
     <row r="227" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A227" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B227">
         <v>24.219999309999999</v>
@@ -7715,7 +7719,7 @@
     </row>
     <row r="228" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A228" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B228">
         <v>24.18000031</v>
@@ -7744,7 +7748,7 @@
     </row>
     <row r="229" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A229" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B229">
         <v>24.399999619999999</v>
@@ -7773,7 +7777,7 @@
     </row>
     <row r="230" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A230" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B230">
         <v>24.579999919999999</v>
@@ -7802,7 +7806,7 @@
     </row>
     <row r="231" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A231" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B231">
         <v>24.579999919999999</v>
@@ -7831,7 +7835,7 @@
     </row>
     <row r="232" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A232" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B232">
         <v>24.260000229999999</v>
@@ -7860,7 +7864,7 @@
     </row>
     <row r="233" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A233" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B233">
         <v>23.920000080000001</v>
@@ -7889,7 +7893,7 @@
     </row>
     <row r="234" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A234" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B234">
         <v>24.100000380000001</v>
@@ -7918,7 +7922,7 @@
     </row>
     <row r="235" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A235" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B235">
         <v>24</v>
@@ -7947,7 +7951,7 @@
     </row>
     <row r="236" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A236" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B236">
         <v>24</v>
@@ -7976,7 +7980,7 @@
     </row>
     <row r="237" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A237" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B237">
         <v>23.840000150000002</v>
@@ -8005,7 +8009,7 @@
     </row>
     <row r="238" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A238" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B238">
         <v>24.020000459999999</v>
@@ -8034,7 +8038,7 @@
     </row>
     <row r="239" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A239" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B239">
         <v>24</v>
@@ -8063,7 +8067,7 @@
     </row>
     <row r="240" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A240" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B240">
         <v>24.079999919999999</v>
@@ -8092,7 +8096,7 @@
     </row>
     <row r="241" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A241" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B241">
         <v>24</v>
@@ -8121,7 +8125,7 @@
     </row>
     <row r="242" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A242" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B242">
         <v>24.020000459999999</v>
@@ -8150,7 +8154,7 @@
     </row>
     <row r="243" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A243" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B243">
         <v>24</v>
@@ -8179,7 +8183,7 @@
     </row>
     <row r="244" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A244" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B244">
         <v>23.879999160000001</v>
@@ -8208,7 +8212,7 @@
     </row>
     <row r="245" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A245" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B245">
         <v>23.879999160000001</v>
@@ -8237,7 +8241,7 @@
     </row>
     <row r="246" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A246" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B246">
         <v>23.840000150000002</v>
@@ -8266,7 +8270,7 @@
     </row>
     <row r="247" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A247" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B247">
         <v>23.600000380000001</v>
@@ -8295,7 +8299,7 @@
     </row>
     <row r="248" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A248" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B248">
         <v>23.479999540000001</v>
@@ -8324,7 +8328,7 @@
     </row>
     <row r="249" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A249" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B249">
         <v>23.059999470000001</v>
@@ -8353,7 +8357,7 @@
     </row>
     <row r="250" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A250" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B250">
         <v>23.13999939</v>
@@ -8382,7 +8386,7 @@
     </row>
     <row r="251" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A251" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B251">
         <v>22.979999540000001</v>

</xml_diff>